<commit_message>
new readme table style
</commit_message>
<xml_diff>
--- a/Test_Documentation/Test_Techniques/Test_Techniques_STA_course.xlsx
+++ b/Test_Documentation/Test_Techniques/Test_Techniques_STA_course.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test_Documentation\Test_Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE19D5C-6912-47B9-812D-D84F71621226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F5AB72-93CC-4AC9-A9B2-E6AB951120F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-4320" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37770" yWindow="-3800" windowWidth="37770" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Task_1.2" sheetId="4" r:id="rId1"/>
+    <sheet name="Test_Techniques_STA_course" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -919,14 +919,68 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -945,9 +999,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -957,62 +1008,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1495,74 +1495,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="38"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="38"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="46"/>
     </row>
     <row r="3" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="38"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="46"/>
     </row>
     <row r="4" spans="1:18" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
@@ -1571,22 +1571,22 @@
       <c r="B4" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="38"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="46"/>
     </row>
     <row r="5" spans="1:18" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
@@ -1595,92 +1595,92 @@
       <c r="B5" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="38"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="46"/>
     </row>
     <row r="6" spans="1:18" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="38"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="46"/>
     </row>
     <row r="7" spans="1:18" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="46"/>
     </row>
     <row r="8" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="39"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="57"/>
     </row>
     <row r="9" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1742,22 +1742,22 @@
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
       <c r="R10" s="19"/>
     </row>
     <row r="11" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -1984,22 +1984,22 @@
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
       <c r="R15" s="19"/>
     </row>
     <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2110,7 +2110,7 @@
       <c r="Q17" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="R17" s="51" t="s">
+      <c r="R17" s="38" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       <c r="Q18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="51"/>
+      <c r="R18" s="38"/>
     </row>
     <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -2220,7 +2220,7 @@
       <c r="Q19" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="R19" s="51"/>
+      <c r="R19" s="38"/>
     </row>
     <row r="20" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
@@ -2290,27 +2290,27 @@
         <f>Q16+25%*Q16-15%*Q16</f>
         <v>165</v>
       </c>
-      <c r="R20" s="51"/>
+      <c r="R20" s="38"/>
     </row>
     <row r="21" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
     </row>
     <row r="22" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
@@ -2343,35 +2343,35 @@
       <c r="J22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="59"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="41"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
     </row>
     <row r="24" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -2404,14 +2404,14 @@
       <c r="J24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
     </row>
     <row r="25" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -2444,14 +2444,14 @@
       <c r="J25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
     </row>
     <row r="26" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
@@ -2484,35 +2484,35 @@
       <c r="J26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="44"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
     </row>
     <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
@@ -2545,14 +2545,14 @@
       <c r="J28" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="38"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
     </row>
     <row r="29" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -2585,14 +2585,14 @@
       <c r="J29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
-      <c r="R29" s="38"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
     </row>
     <row r="30" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
@@ -2625,358 +2625,377 @@
       <c r="J30" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="L30" s="56" t="s">
+      <c r="L30" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="38"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="52"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="46"/>
     </row>
     <row r="31" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="43"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="38"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="61"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="46"/>
     </row>
     <row r="32" spans="1:18" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="38"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="46"/>
     </row>
     <row r="33" spans="1:18" ht="307.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="46"/>
     </row>
     <row r="34" spans="1:18" ht="262.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="46"/>
     </row>
     <row r="35" spans="1:18" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="63"/>
-      <c r="K35" s="63"/>
-      <c r="L35" s="63"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="63"/>
-      <c r="O35" s="63"/>
-      <c r="P35" s="63"/>
-      <c r="Q35" s="63"/>
-      <c r="R35" s="38"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="46"/>
     </row>
     <row r="36" spans="1:18" ht="168" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="52"/>
-      <c r="B36" s="63" t="s">
+      <c r="A36" s="67"/>
+      <c r="B36" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
-      <c r="K36" s="63"/>
-      <c r="L36" s="63"/>
-      <c r="M36" s="63"/>
-      <c r="N36" s="63"/>
-      <c r="O36" s="63"/>
-      <c r="P36" s="63"/>
-      <c r="Q36" s="63"/>
-      <c r="R36" s="38"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="46"/>
     </row>
     <row r="37" spans="1:18" ht="139.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="52"/>
-      <c r="B37" s="63" t="s">
+      <c r="A37" s="67"/>
+      <c r="B37" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="64"/>
-      <c r="M37" s="64"/>
-      <c r="N37" s="64"/>
-      <c r="O37" s="64"/>
-      <c r="P37" s="64"/>
-      <c r="Q37" s="64"/>
-      <c r="R37" s="38"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="48"/>
+      <c r="P37" s="48"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="46"/>
     </row>
     <row r="38" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="55"/>
-      <c r="P38" s="55"/>
-      <c r="Q38" s="55"/>
-      <c r="R38" s="38"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="46"/>
     </row>
     <row r="39" spans="1:18" ht="224.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-      <c r="K39" s="65"/>
-      <c r="L39" s="65"/>
-      <c r="M39" s="65"/>
-      <c r="N39" s="65"/>
-      <c r="O39" s="65"/>
-      <c r="P39" s="65"/>
-      <c r="Q39" s="65"/>
-      <c r="R39" s="38"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="46"/>
     </row>
     <row r="40" spans="1:18" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="46"/>
     </row>
     <row r="41" spans="1:18" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="51"/>
-      <c r="P41" s="51"/>
-      <c r="Q41" s="51"/>
-      <c r="R41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="46"/>
     </row>
     <row r="42" spans="1:18" ht="407.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="43"/>
-      <c r="O42" s="43"/>
-      <c r="P42" s="43"/>
-      <c r="Q42" s="43"/>
-      <c r="R42" s="38"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
+      <c r="K42" s="61"/>
+      <c r="L42" s="61"/>
+      <c r="M42" s="61"/>
+      <c r="N42" s="61"/>
+      <c r="O42" s="61"/>
+      <c r="P42" s="61"/>
+      <c r="Q42" s="61"/>
+      <c r="R42" s="46"/>
     </row>
     <row r="43" spans="1:18" ht="405.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="43"/>
-      <c r="N43" s="43"/>
-      <c r="O43" s="43"/>
-      <c r="P43" s="43"/>
-      <c r="Q43" s="43"/>
-      <c r="R43" s="38"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="61"/>
+      <c r="P43" s="61"/>
+      <c r="Q43" s="61"/>
+      <c r="R43" s="46"/>
     </row>
     <row r="44" spans="1:18" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-      <c r="N44" s="43"/>
-      <c r="O44" s="43"/>
-      <c r="P44" s="43"/>
-      <c r="Q44" s="43"/>
-      <c r="R44" s="38"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="61"/>
+      <c r="O44" s="61"/>
+      <c r="P44" s="61"/>
+      <c r="Q44" s="61"/>
+      <c r="R44" s="46"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="38"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="62"/>
+      <c r="R45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B44:Q44"/>
+    <mergeCell ref="B45:Q45"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A21:Q21"/>
+    <mergeCell ref="K22:Q29"/>
+    <mergeCell ref="A31:Q31"/>
+    <mergeCell ref="A8:Q8"/>
+    <mergeCell ref="B40:Q40"/>
+    <mergeCell ref="B41:Q41"/>
+    <mergeCell ref="B42:Q42"/>
+    <mergeCell ref="B43:Q43"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B5:Q5"/>
     <mergeCell ref="R17:R20"/>
     <mergeCell ref="B23:I23"/>
@@ -2993,25 +3012,6 @@
     <mergeCell ref="B34:Q34"/>
     <mergeCell ref="L30:Q30"/>
     <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="B33:Q33"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B44:Q44"/>
-    <mergeCell ref="B45:Q45"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A21:Q21"/>
-    <mergeCell ref="K22:Q29"/>
-    <mergeCell ref="A31:Q31"/>
-    <mergeCell ref="A8:Q8"/>
-    <mergeCell ref="B40:Q40"/>
-    <mergeCell ref="B41:Q41"/>
-    <mergeCell ref="B42:Q42"/>
-    <mergeCell ref="B43:Q43"/>
-    <mergeCell ref="A35:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
change formating in web pages
</commit_message>
<xml_diff>
--- a/Test_Documentation/Test_Techniques/Test_Techniques_STA_course.xlsx
+++ b/Test_Documentation/Test_Techniques/Test_Techniques_STA_course.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test_Documentation\Test_Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F5AB72-93CC-4AC9-A9B2-E6AB951120F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18B2DE3C-3322-499F-B0F2-FF9805AAEECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37770" yWindow="-3800" windowWidth="37770" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -915,18 +915,69 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -945,12 +996,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -968,51 +1013,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1495,192 +1495,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="46"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="42"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="46"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="46"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="1:18" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="46"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="42"/>
     </row>
     <row r="5" spans="1:18" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="46"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="42"/>
     </row>
     <row r="6" spans="1:18" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="46"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="42"/>
     </row>
     <row r="7" spans="1:18" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38" t="s">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="46"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="42"/>
     </row>
     <row r="8" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="57"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="50"/>
     </row>
     <row r="9" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1742,22 +1742,22 @@
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
       <c r="R10" s="19"/>
     </row>
     <row r="11" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -1984,22 +1984,22 @@
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
       <c r="R15" s="19"/>
     </row>
     <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2110,7 +2110,7 @@
       <c r="Q17" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="R17" s="38" t="s">
+      <c r="R17" s="44" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       <c r="Q18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="38"/>
+      <c r="R18" s="44"/>
     </row>
     <row r="19" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -2220,7 +2220,7 @@
       <c r="Q19" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="R19" s="38"/>
+      <c r="R19" s="44"/>
     </row>
     <row r="20" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
@@ -2290,27 +2290,27 @@
         <f>Q16+25%*Q16-15%*Q16</f>
         <v>165</v>
       </c>
-      <c r="R20" s="38"/>
+      <c r="R20" s="44"/>
     </row>
     <row r="21" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
     </row>
     <row r="22" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
@@ -2343,35 +2343,35 @@
       <c r="J22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="58"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="42"/>
     </row>
     <row r="24" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -2404,14 +2404,14 @@
       <c r="J24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
     </row>
     <row r="25" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -2444,14 +2444,14 @@
       <c r="J25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
     </row>
     <row r="26" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
@@ -2484,35 +2484,35 @@
       <c r="J26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="44"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
-      <c r="P27" s="46"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
     </row>
     <row r="28" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
@@ -2545,14 +2545,14 @@
       <c r="J28" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="46"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
     </row>
     <row r="29" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -2585,14 +2585,14 @@
       <c r="J29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
     </row>
     <row r="30" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
@@ -2625,358 +2625,377 @@
       <c r="J30" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="L30" s="52" t="s">
+      <c r="L30" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-      <c r="P30" s="52"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="46"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="42"/>
     </row>
     <row r="31" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="61"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="61"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="61"/>
-      <c r="P31" s="61"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="46"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="42"/>
     </row>
     <row r="32" spans="1:18" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="46"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="42"/>
     </row>
     <row r="33" spans="1:18" ht="307.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="46"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="42"/>
     </row>
     <row r="34" spans="1:18" ht="262.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="38"/>
-      <c r="R34" s="46"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="42"/>
     </row>
     <row r="35" spans="1:18" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="47"/>
-      <c r="Q35" s="47"/>
-      <c r="R35" s="46"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="62"/>
+      <c r="R35" s="42"/>
     </row>
     <row r="36" spans="1:18" ht="168" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="67"/>
-      <c r="B36" s="47" t="s">
+      <c r="A36" s="45"/>
+      <c r="B36" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="46"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="42"/>
     </row>
     <row r="37" spans="1:18" ht="139.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="67"/>
-      <c r="B37" s="47" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="O37" s="48"/>
-      <c r="P37" s="48"/>
-      <c r="Q37" s="48"/>
-      <c r="R37" s="46"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="Q37" s="63"/>
+      <c r="R37" s="42"/>
     </row>
     <row r="38" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="46"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="64"/>
+      <c r="N38" s="64"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="64"/>
+      <c r="Q38" s="64"/>
+      <c r="R38" s="42"/>
     </row>
     <row r="39" spans="1:18" ht="224.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="51"/>
-      <c r="P39" s="51"/>
-      <c r="Q39" s="51"/>
-      <c r="R39" s="46"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="66"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="66"/>
+      <c r="R39" s="42"/>
     </row>
     <row r="40" spans="1:18" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-      <c r="P40" s="38"/>
-      <c r="Q40" s="38"/>
-      <c r="R40" s="46"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="44"/>
+      <c r="Q40" s="44"/>
+      <c r="R40" s="42"/>
     </row>
     <row r="41" spans="1:18" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
-      <c r="B41" s="38" t="s">
+      <c r="B41" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="46"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="42"/>
     </row>
     <row r="42" spans="1:18" ht="407.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61"/>
-      <c r="N42" s="61"/>
-      <c r="O42" s="61"/>
-      <c r="P42" s="61"/>
-      <c r="Q42" s="61"/>
-      <c r="R42" s="46"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="42"/>
     </row>
     <row r="43" spans="1:18" ht="405.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="61"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="61"/>
-      <c r="N43" s="61"/>
-      <c r="O43" s="61"/>
-      <c r="P43" s="61"/>
-      <c r="Q43" s="61"/>
-      <c r="R43" s="46"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="42"/>
     </row>
     <row r="44" spans="1:18" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61"/>
-      <c r="N44" s="61"/>
-      <c r="O44" s="61"/>
-      <c r="P44" s="61"/>
-      <c r="Q44" s="61"/>
-      <c r="R44" s="46"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="42"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
-      <c r="L45" s="62"/>
-      <c r="M45" s="62"/>
-      <c r="N45" s="62"/>
-      <c r="O45" s="62"/>
-      <c r="P45" s="62"/>
-      <c r="Q45" s="62"/>
-      <c r="R45" s="46"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="36"/>
+      <c r="Q45" s="36"/>
+      <c r="R45" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B15:Q15"/>
+    <mergeCell ref="R21:R45"/>
+    <mergeCell ref="B36:Q36"/>
+    <mergeCell ref="B37:Q37"/>
+    <mergeCell ref="B38:Q38"/>
+    <mergeCell ref="B32:Q32"/>
+    <mergeCell ref="B35:Q35"/>
+    <mergeCell ref="B39:Q39"/>
+    <mergeCell ref="B34:Q34"/>
+    <mergeCell ref="L30:Q30"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B6:Q6"/>
     <mergeCell ref="B44:Q44"/>
     <mergeCell ref="B45:Q45"/>
     <mergeCell ref="B2:Q2"/>
@@ -2993,25 +3012,6 @@
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="J7:Q7"/>
     <mergeCell ref="B33:Q33"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B15:Q15"/>
-    <mergeCell ref="R21:R45"/>
-    <mergeCell ref="B36:Q36"/>
-    <mergeCell ref="B37:Q37"/>
-    <mergeCell ref="B38:Q38"/>
-    <mergeCell ref="B32:Q32"/>
-    <mergeCell ref="B35:Q35"/>
-    <mergeCell ref="B39:Q39"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="B34:Q34"/>
-    <mergeCell ref="L30:Q30"/>
-    <mergeCell ref="B6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>